<commit_message>
Moved referee data; added final paper
</commit_message>
<xml_diff>
--- a/Master Datasets/Player Info Dataset/Player Information v3.xlsx
+++ b/Master Datasets/Player Info Dataset/Player Information v3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erwinmedina/code/finalproject/Data Collection &amp; Processes/Incident Report - Federation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erwinmedina/code/finalproject/Master Datasets/Player Info Dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FEADFB5-B382-554E-A5E1-95703E606FDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C635D2-D8FE-4F41-9106-10A9776E1CBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19300" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21661,8 +21661,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M2889"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1474" zoomScale="136" workbookViewId="0">
-      <selection activeCell="D1485" sqref="D1485"/>
+    <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2034" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F2046" sqref="F2046"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -21670,7 +21671,8 @@
     <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="22" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="5" max="5" width="22" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="24.1640625" customWidth="1"/>
     <col min="7" max="8" width="10.83203125" style="2"/>
     <col min="9" max="11" width="8.83203125" style="2"/>
@@ -98025,5 +98027,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>